<commit_message>
add functions for making line graph
</commit_message>
<xml_diff>
--- a/dmsan/results/RESULTS_AHP_TOPSIS.xlsx
+++ b/dmsan/results/RESULTS_AHP_TOPSIS.xlsx
@@ -32,10 +32,10 @@
     <t>Alternative C</t>
   </si>
   <si>
-    <t>0:1:2:2:1</t>
-  </si>
-  <si>
-    <t>RR, 2Env, 2Econ, S</t>
+    <t>0.25:0.32:0.11:0.19:0.13</t>
+  </si>
+  <si>
+    <t>0.25T, 0.32RR, 0.11Env, 0.19Econ, 0.13S</t>
   </si>
 </sst>
 </file>
@@ -427,13 +427,13 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.5294390373101497</v>
+        <v>0.1682817982949932</v>
       </c>
       <c r="E2">
-        <v>0.5003019992039243</v>
+        <v>0.8156312408875149</v>
       </c>
       <c r="F2">
-        <v>0.121532470759843</v>
+        <v>0.176540863984829</v>
       </c>
     </row>
   </sheetData>
@@ -477,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results with 1000 better selected criteria weights!
</commit_message>
<xml_diff>
--- a/dmsan/results/RESULTS_AHP_TOPSIS.xlsx
+++ b/dmsan/results/RESULTS_AHP_TOPSIS.xlsx
@@ -32,10 +32,10 @@
     <t>Alternative C</t>
   </si>
   <si>
-    <t>0.02:0.01:0.03:0.03:0.91</t>
-  </si>
-  <si>
-    <t>0.02T, 0.01RR, 0.03Env, 0.03Econ, 0.91S</t>
+    <t>0.21:0.07:0.25:0.3:0.17</t>
+  </si>
+  <si>
+    <t>0.21T, 0.07RR, 0.25Env, 0.3Econ, 0.17S</t>
   </si>
 </sst>
 </file>
@@ -427,13 +427,13 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.3813762478735621</v>
+        <v>0.1755158851424245</v>
       </c>
       <c r="E2">
-        <v>0.9783077628436179</v>
+        <v>0.8578473045443887</v>
       </c>
       <c r="F2">
-        <v>0.009442416060179716</v>
+        <v>0.05851766611794292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>